<commit_message>
Entfernen der Inhalte, dass Pkl leer ist
</commit_message>
<xml_diff>
--- a/Ausführung.xlsx
+++ b/Ausführung.xlsx
@@ -566,7 +566,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A295" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -599,17 +599,51 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Klimawandel</t>
+          <t>Belegschaft Lieferkette</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Anpassung an den Klimawandel</t>
+          <t>Arbeitsbedingungen</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>Angemessene Entlohnung</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Biodiversität</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Direkte Ursachen des Biodiversitätsverlusts</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Direkte Ausbeutung</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Externes Thema 1</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Externes Unterthema 1</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Externes Unter-Unterthema 1</t>
         </is>
       </c>
     </row>

</xml_diff>